<commit_message>
add short x carriage version
</commit_message>
<xml_diff>
--- a/HyperRail/Admin/ToOrder.xlsx
+++ b/HyperRail/Admin/ToOrder.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jorian Brusind\Documents\GitHub\PersonalProjects\HyperRail\Admin\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jorian Bruslind\Documents\GitHub\PersonalProjects\HyperRail\Admin\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C8B534D-EB19-4360-9E6B-D142D379DAD6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD0A08FE-2F36-4189-B749-CA8F81FA12CD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-2370" windowWidth="25440" windowHeight="15390" xr2:uid="{FC71E593-D2D1-453C-B906-E07DE7904A14}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{FC71E593-D2D1-453C-B906-E07DE7904A14}"/>
   </bookViews>
   <sheets>
     <sheet name="Overall" sheetId="1" r:id="rId1"/>
@@ -350,87 +350,6 @@
   <dxfs count="17">
     <dxf>
       <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <vertAlign val="baseline"/>
-        <sz val="14"/>
-        <name val="Arial"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="medium">
-          <color rgb="FFCCCCCC"/>
-        </left>
-        <right style="medium">
-          <color rgb="FFCCCCCC"/>
-        </right>
-        <top style="medium">
-          <color rgb="FFCCCCCC"/>
-        </top>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="14"/>
-        <color theme="1"/>
-        <name val="Arial"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="14"/>
-        <color theme="1"/>
-        <name val="Arial"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
         <b val="0"/>
         <i val="0"/>
         <strike val="0"/>
@@ -727,17 +646,11 @@
     </dxf>
     <dxf>
       <font>
-        <b val="0"/>
-        <i val="0"/>
         <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
         <outline val="0"/>
         <shadow val="0"/>
-        <u val="none"/>
         <vertAlign val="baseline"/>
         <sz val="14"/>
-        <color rgb="FF000000"/>
         <name val="Arial"/>
         <family val="2"/>
         <scheme val="none"/>
@@ -811,6 +724,43 @@
         <u val="none"/>
         <vertAlign val="baseline"/>
         <sz val="14"/>
+        <color rgb="FF000000"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="medium">
+          <color rgb="FFCCCCCC"/>
+        </left>
+        <right style="medium">
+          <color rgb="FFCCCCCC"/>
+        </right>
+        <top style="medium">
+          <color rgb="FFCCCCCC"/>
+        </top>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="14"/>
         <color theme="1"/>
         <name val="Arial"/>
         <family val="2"/>
@@ -854,11 +804,61 @@
       </border>
     </dxf>
     <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
       <border outline="0">
         <bottom style="medium">
           <color rgb="FFCCCCCC"/>
         </bottom>
       </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -874,25 +874,25 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{330BDBFC-0040-488F-A14D-50680DEE51A9}" name="Table1" displayName="Table1" ref="A1:L45" totalsRowShown="0" headerRowDxfId="2" dataDxfId="1" headerRowBorderDxfId="16" tableBorderDxfId="15" totalsRowBorderDxfId="14">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{330BDBFC-0040-488F-A14D-50680DEE51A9}" name="Table1" displayName="Table1" ref="A1:L45" totalsRowShown="0" headerRowDxfId="16" dataDxfId="14" headerRowBorderDxfId="15" tableBorderDxfId="13" totalsRowBorderDxfId="12">
   <autoFilter ref="A1:L45" xr:uid="{77151423-1B2A-4470-8822-1A315E897150}"/>
   <tableColumns count="12">
-    <tableColumn id="1" xr3:uid="{CC88C53F-726A-425D-90A5-C838FFD1FC8D}" name="Date needed" dataDxfId="13"/>
-    <tableColumn id="2" xr3:uid="{8ED03E7E-506A-4EF5-94A3-A24D108E43EE}" name="Shipping" dataDxfId="12"/>
-    <tableColumn id="3" xr3:uid="{1DB284AE-77CA-42C2-8DAB-D69BC223494F}" name="Requester" dataDxfId="11"/>
-    <tableColumn id="4" xr3:uid="{D50BF9C3-B57F-43FD-B322-8D5833B9F22D}" name="Source" dataDxfId="0" dataCellStyle="Hyperlink">
+    <tableColumn id="1" xr3:uid="{CC88C53F-726A-425D-90A5-C838FFD1FC8D}" name="Date needed" dataDxfId="11"/>
+    <tableColumn id="2" xr3:uid="{8ED03E7E-506A-4EF5-94A3-A24D108E43EE}" name="Shipping" dataDxfId="10"/>
+    <tableColumn id="3" xr3:uid="{1DB284AE-77CA-42C2-8DAB-D69BC223494F}" name="Requester" dataDxfId="9"/>
+    <tableColumn id="4" xr3:uid="{D50BF9C3-B57F-43FD-B322-8D5833B9F22D}" name="Source" dataDxfId="8" dataCellStyle="Hyperlink">
       <calculatedColumnFormula>HYPERLINK("https://www.amazon.com/AmazonBasics-Printer-Filament-1-75mm-Black/dp/B07T2QZYS1/ref=sr_1_15?dchild=1&amp;keywords=PETG&amp;qid=1617819005&amp;sr=8-15&amp;th=1","Amazon")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{D8F29473-C36E-4E86-8820-F79741720813}" name="Description" dataDxfId="10"/>
-    <tableColumn id="6" xr3:uid="{CBA968D8-9A82-41B1-955C-4E21934861A9}" name="Units" dataDxfId="9"/>
-    <tableColumn id="7" xr3:uid="{98BDFD10-EB34-4902-BE4B-F77503488929}" name="Part number" dataDxfId="8"/>
-    <tableColumn id="8" xr3:uid="{951205BB-92C6-448D-BE14-2265BFBB63BF}" name="Price/unit" dataDxfId="7" dataCellStyle="Currency"/>
-    <tableColumn id="9" xr3:uid="{8A166005-67D3-4E42-A96E-A93874D808EF}" name="Total" dataDxfId="6" dataCellStyle="Currency">
+    <tableColumn id="5" xr3:uid="{D8F29473-C36E-4E86-8820-F79741720813}" name="Description" dataDxfId="7"/>
+    <tableColumn id="6" xr3:uid="{CBA968D8-9A82-41B1-955C-4E21934861A9}" name="Units" dataDxfId="6"/>
+    <tableColumn id="7" xr3:uid="{98BDFD10-EB34-4902-BE4B-F77503488929}" name="Part number" dataDxfId="5"/>
+    <tableColumn id="8" xr3:uid="{951205BB-92C6-448D-BE14-2265BFBB63BF}" name="Price/unit" dataDxfId="4" dataCellStyle="Currency"/>
+    <tableColumn id="9" xr3:uid="{8A166005-67D3-4E42-A96E-A93874D808EF}" name="Total" dataDxfId="3" dataCellStyle="Currency">
       <calculatedColumnFormula>Table1[[#This Row],[Price/unit]]*Table1[[#This Row],[Units]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="10" xr3:uid="{896DDBB2-F53B-4A39-8EB5-A975A4049ECA}" name="Purpose: X for Y" dataDxfId="5"/>
-    <tableColumn id="11" xr3:uid="{1FCCE8EF-0FF7-464C-9451-A29EF0846838}" name="Notes" dataDxfId="4"/>
-    <tableColumn id="12" xr3:uid="{28CDBEEF-6DF9-4CFD-A5B4-4921F498468A}" name="Project" dataDxfId="3"/>
+    <tableColumn id="10" xr3:uid="{896DDBB2-F53B-4A39-8EB5-A975A4049ECA}" name="Purpose: X for Y" dataDxfId="2"/>
+    <tableColumn id="11" xr3:uid="{1FCCE8EF-0FF7-464C-9451-A29EF0846838}" name="Notes" dataDxfId="1"/>
+    <tableColumn id="12" xr3:uid="{28CDBEEF-6DF9-4CFD-A5B4-4921F498468A}" name="Project" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1197,7 +1197,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{40B72B52-33F4-4B8E-8548-DD772DC25706}">
   <dimension ref="A1:P45"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="G15" sqref="G15"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
update assembly with bearings
</commit_message>
<xml_diff>
--- a/HyperRail/Admin/ToOrder.xlsx
+++ b/HyperRail/Admin/ToOrder.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jorian Bruslind\Documents\GitHub\PersonalProjects\HyperRail\Admin\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jorian Brusind\Documents\GitHub\PersonalProjects\HyperRail\Admin\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD0A08FE-2F36-4189-B749-CA8F81FA12CD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{324E0090-C40F-4FDE-AEE0-222DBDF247A8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{FC71E593-D2D1-453C-B906-E07DE7904A14}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{FC71E593-D2D1-453C-B906-E07DE7904A14}"/>
   </bookViews>
   <sheets>
     <sheet name="Overall" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="164" uniqueCount="82">
   <si>
     <t>Date needed</t>
   </si>
@@ -78,106 +78,208 @@
     <t>Jorian Bruslind</t>
   </si>
   <si>
-    <t>Amazon Basics PETG</t>
-  </si>
-  <si>
-    <t>PETG175GY21000C</t>
-  </si>
-  <si>
-    <t>Weatherproof Printing</t>
-  </si>
-  <si>
     <t>HyperRail</t>
   </si>
   <si>
     <t>SubTotal</t>
   </si>
   <si>
-    <t>40x40 Aluminum Extrusion - 2m</t>
-  </si>
-  <si>
-    <t>Extended Y Axis</t>
-  </si>
-  <si>
-    <t>40x40 Aluminum Extrusion - 1.5m</t>
-  </si>
-  <si>
-    <t>HFS5-4040-1500</t>
-  </si>
-  <si>
-    <t>12pc Pulley Wheels</t>
-  </si>
-  <si>
-    <t>B07KPWJ3ZC</t>
-  </si>
-  <si>
-    <t>HFS5-2020-2892</t>
-  </si>
-  <si>
-    <t>Z Axis Height</t>
-  </si>
-  <si>
-    <t>More supporting wheels</t>
-  </si>
-  <si>
-    <t>X axis strut supports</t>
-  </si>
-  <si>
-    <t>Plastic Case - EBOX Assembly</t>
-  </si>
-  <si>
-    <t>SE300,OR</t>
-  </si>
-  <si>
-    <t>Ebox for electronics protection</t>
-  </si>
-  <si>
-    <t>B08HSXGZ5R</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Ebox Assembly (Ethernet inserts) </t>
-  </si>
-  <si>
-    <t>Ethernet Cable Glands - 5pk</t>
-  </si>
-  <si>
-    <t>GT2 Rubber Timing Belt - 10m</t>
-  </si>
-  <si>
-    <t>B08974S1CC</t>
-  </si>
-  <si>
-    <t>Dual Belt Upgrades</t>
-  </si>
-  <si>
-    <t>https://www.amazon.com/Seahorse-Protective-Case-Foam-Orange/dp/B001A1PT9A/ref=pd_lpo_card_1?pd_rd_i=B001A1PT9A&amp;th=1</t>
-  </si>
-  <si>
-    <t>https://amzn.to/3iH1E9Q</t>
-  </si>
-  <si>
-    <t>https://www.amazon.com/Printing-Zeelo-Fiberglass-Rostock-Printers/dp/B08974S1CC/ref=sr_1_7?dchild=1&amp;keywords=Gt2&amp;qid=1623868289&amp;rnid=2941120011&amp;s=industrial&amp;sr=1-7</t>
-  </si>
-  <si>
-    <t>https://bit.ly/3gxVAz7</t>
-  </si>
-  <si>
-    <t>https://www.amazon.com/AFUNTA-Plastic-Bearings-Printer-Compatible/dp/B07KPWJ3ZC/ref=sr_1_3?dchild=1&amp;keywords=delrin+wheels&amp;qid=1623787367&amp;sr=8-3</t>
-  </si>
-  <si>
-    <t>https://bit.ly/2RXyo3x</t>
-  </si>
-  <si>
-    <t>https://bit.ly/2TA86oo</t>
-  </si>
-  <si>
-    <t>https://www.amazon.com/AmazonBasics-Printer-Filament-1-75mm-Black/dp/B07T6W63MY/ref=sr_1_10?dchild=1&amp;keywords=PETG&amp;qid=1623866514&amp;sr=8-10&amp;th=1</t>
-  </si>
-  <si>
-    <t>HFS5-4040-2000</t>
-  </si>
-  <si>
-    <t>20x20 Aluminum Extrusion - 1.928m</t>
+    <t>B20-5M-MPS</t>
+  </si>
+  <si>
+    <t>20mm HTD5 Belt</t>
+  </si>
+  <si>
+    <t>Custom cut belt used for lower track length</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Price listed online is per ft </t>
+  </si>
+  <si>
+    <t>650mm HTD5 closed loop Belt</t>
+  </si>
+  <si>
+    <t>B650-5M-09CPS</t>
+  </si>
+  <si>
+    <t>Closed loop belt for pulley to interface to lower track</t>
+  </si>
+  <si>
+    <t>Steel cord HTD5 profile</t>
+  </si>
+  <si>
+    <t>3M VHB Tape LSE-160WF 1</t>
+  </si>
+  <si>
+    <t>LSE-160WF 1"</t>
+  </si>
+  <si>
+    <t>Adhesive for static belt layer</t>
+  </si>
+  <si>
+    <t>Price for 5yd roll</t>
+  </si>
+  <si>
+    <t>1276-1033-1-ND</t>
+  </si>
+  <si>
+    <t>478-7019-1-ND</t>
+  </si>
+  <si>
+    <t>1276-3179-1-ND</t>
+  </si>
+  <si>
+    <t>609-1046-ND</t>
+  </si>
+  <si>
+    <t>A128140-ND</t>
+  </si>
+  <si>
+    <t>ED2637-ND</t>
+  </si>
+  <si>
+    <t>311-20.0KHRCT-ND</t>
+  </si>
+  <si>
+    <t>RMCF0603FT4K70CT-ND</t>
+  </si>
+  <si>
+    <t>A130089CT-ND</t>
+  </si>
+  <si>
+    <t>450-1790-1-ND</t>
+  </si>
+  <si>
+    <t>641-1326-1-ND</t>
+  </si>
+  <si>
+    <t>P19261CT-ND</t>
+  </si>
+  <si>
+    <t>490-2650-1-ND</t>
+  </si>
+  <si>
+    <t>1276-6736-1-ND</t>
+  </si>
+  <si>
+    <t>CAP CER 0.1UF 50V X7R 0603</t>
+  </si>
+  <si>
+    <t>CAP CER 0.022UF 50V X7R 0603</t>
+  </si>
+  <si>
+    <t>CAP CER 4.7UF 50V X7R 1206</t>
+  </si>
+  <si>
+    <t>CONN MOD JACK 8P8C R/A UNSHLD</t>
+  </si>
+  <si>
+    <t>CONN MOD JACK 6P4C R/A UNSHLD</t>
+  </si>
+  <si>
+    <t>TERM BLK 4POS SIDE ENT 3.5MM PCB</t>
+  </si>
+  <si>
+    <t>RES SMD 20K OHM 1% 1/10W 0603</t>
+  </si>
+  <si>
+    <t>RES 4.7K OHM 1% 1/10W 0603</t>
+  </si>
+  <si>
+    <t>CRGCQ 0603 470R 5%</t>
+  </si>
+  <si>
+    <t>SWITCH SLIDE DIP SPST 25MA 24V</t>
+  </si>
+  <si>
+    <t>DIODE SCHOTTKY 20V 500MA SOD123</t>
+  </si>
+  <si>
+    <t>RES 0.11 OHM 5% 1/2W 0805</t>
+  </si>
+  <si>
+    <t>TRIMMER 20K OHM 0.25W J LEAD TOP</t>
+  </si>
+  <si>
+    <t>CAP CER 10UF 50V X5R 1206</t>
+  </si>
+  <si>
+    <t>Integrated Step Driver PCBs</t>
+  </si>
+  <si>
+    <t>Non-Isolated DC/DC Converters</t>
+  </si>
+  <si>
+    <t>TMC2209 Step Stick Drivers</t>
+  </si>
+  <si>
+    <t xml:space="preserve">595-LMZM23601V5SILT </t>
+  </si>
+  <si>
+    <t>‎ B07YW7BM68</t>
+  </si>
+  <si>
+    <t>Digikey out of stock. Need from Mouser</t>
+  </si>
+  <si>
+    <t>Will salvage TMC2209 ICs from these boards</t>
+  </si>
+  <si>
+    <t>30mm M5 Standoffs</t>
+  </si>
+  <si>
+    <t>732-10632-ND‎</t>
+  </si>
+  <si>
+    <t>X Carriage Assembly</t>
+  </si>
+  <si>
+    <t>GT2 Idler Pulley 20 Toothless 5mm Bore 10mm Width</t>
+  </si>
+  <si>
+    <t>B07BPHRSN5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">F696ZZ Flanged Ball Bearing </t>
+  </si>
+  <si>
+    <t>F696ZZ</t>
+  </si>
+  <si>
+    <t>C1, C2, C9, C11, C12_ INTEGRATED</t>
+  </si>
+  <si>
+    <t>VD1, VD2_ INTEGRATED</t>
+  </si>
+  <si>
+    <t>SW1_INTEGRATED</t>
+  </si>
+  <si>
+    <t>J2_ INTEGRATED</t>
+  </si>
+  <si>
+    <t>J3_ INTEGRATED</t>
+  </si>
+  <si>
+    <t>J1_ INTEGRATED</t>
+  </si>
+  <si>
+    <t>R1, R2_ INTEGRATED</t>
+  </si>
+  <si>
+    <t>R4_ INTEGRATED</t>
+  </si>
+  <si>
+    <t>R3, R5, R6, R7, R8, R9_ INTEGRATED</t>
+  </si>
+  <si>
+    <t>C5_ INTEGRATED</t>
+  </si>
+  <si>
+    <t>C3, C4, C6, C7, C10_ INTEGRATED</t>
+  </si>
+  <si>
+    <t>C8_ INTEGRATED</t>
   </si>
 </sst>
 </file>
@@ -187,7 +289,7 @@
   <numFmts count="1">
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -236,13 +338,23 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="5">
@@ -304,12 +416,13 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="3">
+  <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -340,12 +453,29 @@
     <xf numFmtId="44" fontId="4" fillId="0" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="44" fontId="4" fillId="2" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="44" fontId="4" fillId="2" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="3">
+  <cellStyles count="4">
     <cellStyle name="Currency" xfId="1" builtinId="4"/>
     <cellStyle name="Hyperlink" xfId="2" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal 2" xfId="3" xr:uid="{61AEB7E4-7DEA-45EE-A59E-5833FAE85740}"/>
   </cellStyles>
   <dxfs count="17">
     <dxf>
@@ -874,8 +1004,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{330BDBFC-0040-488F-A14D-50680DEE51A9}" name="Table1" displayName="Table1" ref="A1:L45" totalsRowShown="0" headerRowDxfId="16" dataDxfId="14" headerRowBorderDxfId="15" tableBorderDxfId="13" totalsRowBorderDxfId="12">
-  <autoFilter ref="A1:L45" xr:uid="{77151423-1B2A-4470-8822-1A315E897150}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{330BDBFC-0040-488F-A14D-50680DEE51A9}" name="Table1" displayName="Table1" ref="A1:L44" totalsRowShown="0" headerRowDxfId="16" dataDxfId="14" headerRowBorderDxfId="15" tableBorderDxfId="13" totalsRowBorderDxfId="12">
+  <autoFilter ref="A1:L44" xr:uid="{77151423-1B2A-4470-8822-1A315E897150}"/>
   <tableColumns count="12">
     <tableColumn id="1" xr3:uid="{CC88C53F-726A-425D-90A5-C838FFD1FC8D}" name="Date needed" dataDxfId="11"/>
     <tableColumn id="2" xr3:uid="{8ED03E7E-506A-4EF5-94A3-A24D108E43EE}" name="Shipping" dataDxfId="10"/>
@@ -1195,10 +1325,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{40B72B52-33F4-4B8E-8548-DD772DC25706}">
-  <dimension ref="A1:P45"/>
+  <dimension ref="A1:P44"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G15" sqref="G15"/>
+      <selection activeCell="J25" sqref="J25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.25"/>
@@ -1268,40 +1398,40 @@
         <v>12</v>
       </c>
       <c r="D2" s="1" t="str">
-        <f>HYPERLINK("https://www.amazon.com/AmazonBasics-Printer-Filament-1-75mm-Black/dp/B07T6W63MY/ref=sr_1_10?dchild=1&amp;keywords=PETG&amp;qid=1623866514&amp;sr=8-10&amp;th=1","Amazon")</f>
-        <v>Amazon</v>
+        <f>HYPERLINK("https://shop.polybelt.com/20-5M-Open-End-Belt-Roll-Polyurethane-with-Steel-Cords-B20-5M-MPS.htm","PolyBelt")</f>
+        <v>PolyBelt</v>
       </c>
       <c r="E2" s="6" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="F2" s="9">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="G2" s="6" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="H2" s="10">
-        <v>20.04</v>
+        <v>5.4</v>
       </c>
       <c r="I2" s="10">
         <f>Table1[[#This Row],[Price/unit]]*Table1[[#This Row],[Units]]</f>
-        <v>40.08</v>
+        <v>32.400000000000006</v>
       </c>
       <c r="J2" s="6" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="K2" s="1" t="s">
-        <v>45</v>
+        <v>19</v>
       </c>
       <c r="L2" s="6" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="O2" s="11" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="P2" s="12">
         <f>SUM(Table1[Total])</f>
-        <v>394.85</v>
+        <v>206.52700000000002</v>
       </c>
     </row>
     <row r="3" spans="1:16" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1313,33 +1443,33 @@
         <v>12</v>
       </c>
       <c r="D3" s="1" t="str">
-        <f>HYPERLINK("https://bit.ly/3q1RzWx","Misumi")</f>
-        <v>Misumi</v>
+        <f>HYPERLINK("https://shop.polybelt.com/650-5m-09-Urethane-Steel-Timing-Belt-130-Tooth-B650-5M-09CPS.htm","PolyBelt")</f>
+        <v>PolyBelt</v>
       </c>
       <c r="E3" s="6" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="F3" s="9">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G3" s="6" t="s">
-        <v>46</v>
+        <v>21</v>
       </c>
       <c r="H3" s="10">
-        <v>35.4</v>
+        <v>13.5</v>
       </c>
       <c r="I3" s="10">
-        <f>Table1[[#This Row],[Units]]*Table1[[#This Row],[Price/unit]]</f>
-        <v>106.19999999999999</v>
+        <f>Table1[[#This Row],[Price/unit]]*Table1[[#This Row],[Units]]</f>
+        <v>27</v>
       </c>
       <c r="J3" s="6" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="K3" s="1" t="s">
-        <v>44</v>
+        <v>23</v>
       </c>
       <c r="L3" s="6" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
     </row>
     <row r="4" spans="1:16" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1351,422 +1481,752 @@
         <v>12</v>
       </c>
       <c r="D4" s="1" t="str">
-        <f>HYPERLINK("https://bit.ly/2RXyo3x","Misumi")</f>
-        <v>Misumi</v>
+        <f>HYPERLINK("https://amzn.to/2XfDoTI","Amazon")</f>
+        <v>Amazon</v>
       </c>
       <c r="E4" s="6" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="F4" s="9">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G4" s="13" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="H4" s="14">
-        <v>26.55</v>
+        <v>25.39</v>
       </c>
       <c r="I4" s="10">
-        <f>Table1[[#This Row],[Units]]*Table1[[#This Row],[Price/unit]]</f>
-        <v>53.1</v>
+        <f>Table1[[#This Row],[Price/unit]]*Table1[[#This Row],[Units]]</f>
+        <v>25.39</v>
       </c>
       <c r="J4" s="6" t="s">
         <v>26</v>
       </c>
       <c r="K4" s="1" t="s">
-        <v>43</v>
+        <v>27</v>
       </c>
       <c r="L4" s="6" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
     </row>
     <row r="5" spans="1:16" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="6"/>
-      <c r="B5" s="7" t="s">
+      <c r="B5" s="18" t="s">
         <v>13</v>
       </c>
-      <c r="C5" s="7" t="s">
+      <c r="C5" s="18" t="s">
         <v>12</v>
       </c>
-      <c r="D5" s="1" t="str">
-        <f>HYPERLINK("https://www.amazon.com/AFUNTA-Plastic-Bearings-Printer-Compatible/dp/B07KPWJ3ZC/ref=sr_1_3?dchild=1&amp;keywords=delrin+wheels&amp;qid=1623787367&amp;sr=8-3","Amazon")</f>
-        <v>Amazon</v>
-      </c>
-      <c r="E5" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="F5" s="9">
-        <v>3</v>
-      </c>
-      <c r="G5" s="13" t="s">
-        <v>24</v>
-      </c>
-      <c r="H5" s="10">
-        <v>11.59</v>
-      </c>
-      <c r="I5" s="10">
-        <f>Table1[[#This Row],[Units]]*Table1[[#This Row],[Price/unit]]</f>
-        <v>34.769999999999996</v>
-      </c>
-      <c r="J5" s="6" t="s">
-        <v>27</v>
-      </c>
-      <c r="K5" s="1" t="s">
+      <c r="D5" s="19" t="str">
+        <f>HYPERLINK("https://www.digikey.com/short/b3nttrc0", "Digikey Cart")</f>
+        <v>Digikey Cart</v>
+      </c>
+      <c r="E5" s="20" t="s">
         <v>42</v>
       </c>
+      <c r="F5" s="21">
+        <v>15</v>
+      </c>
+      <c r="G5" s="22" t="s">
+        <v>28</v>
+      </c>
+      <c r="H5" s="23">
+        <v>4.3999999999999997E-2</v>
+      </c>
+      <c r="I5" s="23">
+        <f>Table1[[#This Row],[Price/unit]]*Table1[[#This Row],[Units]]</f>
+        <v>0.65999999999999992</v>
+      </c>
+      <c r="J5" s="20" t="s">
+        <v>56</v>
+      </c>
+      <c r="K5" s="19" t="s">
+        <v>70</v>
+      </c>
       <c r="L5" s="6" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
     </row>
     <row r="6" spans="1:16" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="6"/>
-      <c r="B6" s="7" t="s">
+      <c r="B6" s="18" t="s">
         <v>13</v>
       </c>
-      <c r="C6" s="7" t="s">
+      <c r="C6" s="18" t="s">
         <v>12</v>
       </c>
-      <c r="D6" s="1" t="str">
-        <f>HYPERLINK("https://bit.ly/3gxVAz7","Misumi")</f>
-        <v>Misumi</v>
-      </c>
-      <c r="E6" s="6" t="s">
-        <v>47</v>
-      </c>
-      <c r="F6" s="9">
-        <v>6</v>
-      </c>
-      <c r="G6" s="6" t="s">
-        <v>25</v>
-      </c>
-      <c r="H6" s="10">
-        <v>12.72</v>
-      </c>
-      <c r="I6" s="10">
-        <f>Table1[[#This Row],[Units]]*Table1[[#This Row],[Price/unit]]</f>
-        <v>76.320000000000007</v>
-      </c>
-      <c r="J6" s="6" t="s">
-        <v>28</v>
-      </c>
-      <c r="K6" s="1" t="s">
-        <v>41</v>
+      <c r="D6" s="19" t="str">
+        <f t="shared" ref="D6:D19" si="0">HYPERLINK("https://www.digikey.com/short/b3nttrc0", "Digikey Cart")</f>
+        <v>Digikey Cart</v>
+      </c>
+      <c r="E6" s="20" t="s">
+        <v>43</v>
+      </c>
+      <c r="F6" s="21">
+        <v>3</v>
+      </c>
+      <c r="G6" s="20" t="s">
+        <v>29</v>
+      </c>
+      <c r="H6" s="23">
+        <v>0.11</v>
+      </c>
+      <c r="I6" s="23">
+        <f>Table1[[#This Row],[Price/unit]]*Table1[[#This Row],[Units]]</f>
+        <v>0.33</v>
+      </c>
+      <c r="J6" s="20" t="s">
+        <v>56</v>
+      </c>
+      <c r="K6" s="19" t="s">
+        <v>71</v>
       </c>
       <c r="L6" s="6" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
     </row>
     <row r="7" spans="1:16" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="15"/>
-      <c r="B7" s="7" t="s">
+      <c r="B7" s="18" t="s">
         <v>13</v>
       </c>
-      <c r="C7" s="7" t="s">
+      <c r="C7" s="18" t="s">
         <v>12</v>
       </c>
-      <c r="D7" s="1" t="str">
-        <f>HYPERLINK("https://www.amazon.com/Seahorse-Protective-Case-Foam-Orange/dp/B001A1PT9A/ref=pd_lpo_card_1?pd_rd_i=B001A1PT9A&amp;th=1","Amazon")</f>
-        <v>Amazon</v>
-      </c>
-      <c r="E7" s="15" t="s">
-        <v>29</v>
-      </c>
-      <c r="F7" s="16">
-        <v>1</v>
-      </c>
-      <c r="G7" s="15" t="s">
+      <c r="D7" s="19" t="str">
+        <f t="shared" si="0"/>
+        <v>Digikey Cart</v>
+      </c>
+      <c r="E7" s="24" t="s">
+        <v>44</v>
+      </c>
+      <c r="F7" s="25">
+        <v>3</v>
+      </c>
+      <c r="G7" s="24" t="s">
         <v>30</v>
       </c>
-      <c r="H7" s="17">
-        <v>31.41</v>
-      </c>
-      <c r="I7" s="10">
-        <f>Table1[[#This Row],[Units]]*Table1[[#This Row],[Price/unit]]</f>
-        <v>31.41</v>
-      </c>
-      <c r="J7" s="6" t="s">
-        <v>31</v>
-      </c>
-      <c r="K7" s="18" t="s">
-        <v>38</v>
+      <c r="H7" s="26">
+        <v>0.42</v>
+      </c>
+      <c r="I7" s="23">
+        <f>Table1[[#This Row],[Price/unit]]*Table1[[#This Row],[Units]]</f>
+        <v>1.26</v>
+      </c>
+      <c r="J7" s="20" t="s">
+        <v>56</v>
+      </c>
+      <c r="K7" s="19" t="s">
+        <v>72</v>
       </c>
       <c r="L7" s="6" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
     </row>
     <row r="8" spans="1:16" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="15"/>
-      <c r="B8" s="7" t="s">
+      <c r="B8" s="18" t="s">
         <v>13</v>
       </c>
-      <c r="C8" s="7" t="s">
+      <c r="C8" s="18" t="s">
         <v>12</v>
       </c>
-      <c r="D8" s="1" t="str">
-        <f>HYPERLINK("https://amzn.to/3iH1E9Q","Amazon")</f>
-        <v>Amazon</v>
-      </c>
-      <c r="E8" s="15" t="s">
-        <v>34</v>
-      </c>
-      <c r="F8" s="16">
-        <v>1</v>
-      </c>
-      <c r="G8" s="15" t="s">
-        <v>32</v>
-      </c>
-      <c r="H8" s="17">
-        <v>26.99</v>
-      </c>
-      <c r="I8" s="10">
-        <f>Table1[[#This Row],[Units]]*Table1[[#This Row],[Price/unit]]</f>
-        <v>26.99</v>
-      </c>
-      <c r="J8" s="6" t="s">
-        <v>33</v>
-      </c>
-      <c r="K8" s="18" t="s">
-        <v>39</v>
+      <c r="D8" s="19" t="str">
+        <f t="shared" si="0"/>
+        <v>Digikey Cart</v>
+      </c>
+      <c r="E8" s="24" t="s">
+        <v>45</v>
+      </c>
+      <c r="F8" s="25">
+        <v>3</v>
+      </c>
+      <c r="G8" s="24" t="s">
+        <v>31</v>
+      </c>
+      <c r="H8" s="26">
+        <v>0.72</v>
+      </c>
+      <c r="I8" s="23">
+        <f>Table1[[#This Row],[Price/unit]]*Table1[[#This Row],[Units]]</f>
+        <v>2.16</v>
+      </c>
+      <c r="J8" s="20" t="s">
+        <v>56</v>
+      </c>
+      <c r="K8" s="19" t="s">
+        <v>73</v>
       </c>
       <c r="L8" s="6" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
     </row>
     <row r="9" spans="1:16" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="15"/>
-      <c r="B9" s="7" t="s">
+      <c r="B9" s="18" t="s">
         <v>13</v>
       </c>
-      <c r="C9" s="7" t="s">
+      <c r="C9" s="18" t="s">
         <v>12</v>
       </c>
-      <c r="D9" s="1" t="str">
-        <f>HYPERLINK("https://www.amazon.com/Printing-Zeelo-Fiberglass-Rostock-Printers/dp/B08974S1CC/ref=sr_1_7?dchild=1&amp;keywords=Gt2&amp;qid=1623868289&amp;rnid=2941120011&amp;s=industrial&amp;sr=1-7","Amazon")</f>
-        <v>Amazon</v>
-      </c>
-      <c r="E9" s="15" t="s">
-        <v>35</v>
-      </c>
-      <c r="F9" s="16">
-        <v>2</v>
-      </c>
-      <c r="G9" s="13" t="s">
-        <v>36</v>
-      </c>
-      <c r="H9" s="17">
-        <v>12.99</v>
-      </c>
-      <c r="I9" s="10">
-        <f>Table1[[#This Row],[Units]]*Table1[[#This Row],[Price/unit]]</f>
-        <v>25.98</v>
-      </c>
-      <c r="J9" s="6" t="s">
-        <v>37</v>
-      </c>
-      <c r="K9" s="18" t="s">
-        <v>40</v>
+      <c r="D9" s="19" t="str">
+        <f t="shared" si="0"/>
+        <v>Digikey Cart</v>
+      </c>
+      <c r="E9" s="24" t="s">
+        <v>46</v>
+      </c>
+      <c r="F9" s="25">
+        <v>3</v>
+      </c>
+      <c r="G9" s="22" t="s">
+        <v>32</v>
+      </c>
+      <c r="H9" s="26">
+        <v>1.05</v>
+      </c>
+      <c r="I9" s="23">
+        <f>Table1[[#This Row],[Price/unit]]*Table1[[#This Row],[Units]]</f>
+        <v>3.1500000000000004</v>
+      </c>
+      <c r="J9" s="20" t="s">
+        <v>56</v>
+      </c>
+      <c r="K9" s="19" t="s">
+        <v>74</v>
       </c>
       <c r="L9" s="6" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
     </row>
     <row r="10" spans="1:16" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="15"/>
-      <c r="B10" s="7"/>
-      <c r="C10" s="7"/>
-      <c r="D10" s="8"/>
-      <c r="E10" s="15"/>
-      <c r="F10" s="16"/>
-      <c r="G10" s="15"/>
-      <c r="H10" s="17"/>
-      <c r="I10" s="10"/>
-      <c r="J10" s="6"/>
-      <c r="K10" s="15"/>
-      <c r="L10" s="6"/>
+      <c r="B10" s="18" t="s">
+        <v>13</v>
+      </c>
+      <c r="C10" s="18" t="s">
+        <v>12</v>
+      </c>
+      <c r="D10" s="19" t="str">
+        <f t="shared" si="0"/>
+        <v>Digikey Cart</v>
+      </c>
+      <c r="E10" s="24" t="s">
+        <v>47</v>
+      </c>
+      <c r="F10" s="25">
+        <v>3</v>
+      </c>
+      <c r="G10" s="24" t="s">
+        <v>33</v>
+      </c>
+      <c r="H10" s="26">
+        <v>1.06</v>
+      </c>
+      <c r="I10" s="23">
+        <f>Table1[[#This Row],[Price/unit]]*Table1[[#This Row],[Units]]</f>
+        <v>3.18</v>
+      </c>
+      <c r="J10" s="20" t="s">
+        <v>56</v>
+      </c>
+      <c r="K10" s="19" t="s">
+        <v>75</v>
+      </c>
+      <c r="L10" s="6" t="s">
+        <v>14</v>
+      </c>
     </row>
     <row r="11" spans="1:16" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="15"/>
-      <c r="B11" s="7"/>
-      <c r="C11" s="7"/>
-      <c r="D11" s="8"/>
-      <c r="E11" s="15"/>
-      <c r="F11" s="16"/>
-      <c r="G11" s="15"/>
-      <c r="H11" s="17"/>
-      <c r="I11" s="10"/>
-      <c r="J11" s="6"/>
-      <c r="K11" s="15"/>
-      <c r="L11" s="6"/>
+      <c r="B11" s="18" t="s">
+        <v>13</v>
+      </c>
+      <c r="C11" s="18" t="s">
+        <v>12</v>
+      </c>
+      <c r="D11" s="19" t="str">
+        <f t="shared" si="0"/>
+        <v>Digikey Cart</v>
+      </c>
+      <c r="E11" s="24" t="s">
+        <v>48</v>
+      </c>
+      <c r="F11" s="25">
+        <v>18</v>
+      </c>
+      <c r="G11" s="24" t="s">
+        <v>34</v>
+      </c>
+      <c r="H11" s="26">
+        <v>2.4E-2</v>
+      </c>
+      <c r="I11" s="23">
+        <f>Table1[[#This Row],[Price/unit]]*Table1[[#This Row],[Units]]</f>
+        <v>0.432</v>
+      </c>
+      <c r="J11" s="20" t="s">
+        <v>56</v>
+      </c>
+      <c r="K11" s="19" t="s">
+        <v>76</v>
+      </c>
+      <c r="L11" s="6" t="s">
+        <v>14</v>
+      </c>
     </row>
     <row r="12" spans="1:16" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="15"/>
-      <c r="B12" s="7"/>
-      <c r="C12" s="7"/>
-      <c r="D12" s="8"/>
-      <c r="E12" s="15"/>
-      <c r="F12" s="16"/>
-      <c r="G12" s="15"/>
-      <c r="H12" s="17"/>
-      <c r="I12" s="10"/>
-      <c r="J12" s="6"/>
-      <c r="K12" s="15"/>
-      <c r="L12" s="6"/>
+      <c r="B12" s="18" t="s">
+        <v>13</v>
+      </c>
+      <c r="C12" s="18" t="s">
+        <v>12</v>
+      </c>
+      <c r="D12" s="19" t="str">
+        <f t="shared" si="0"/>
+        <v>Digikey Cart</v>
+      </c>
+      <c r="E12" s="24" t="s">
+        <v>49</v>
+      </c>
+      <c r="F12" s="25">
+        <v>3</v>
+      </c>
+      <c r="G12" s="24" t="s">
+        <v>35</v>
+      </c>
+      <c r="H12" s="26">
+        <v>0.1</v>
+      </c>
+      <c r="I12" s="23">
+        <f>Table1[[#This Row],[Price/unit]]*Table1[[#This Row],[Units]]</f>
+        <v>0.30000000000000004</v>
+      </c>
+      <c r="J12" s="20" t="s">
+        <v>56</v>
+      </c>
+      <c r="K12" s="19" t="s">
+        <v>77</v>
+      </c>
+      <c r="L12" s="6" t="s">
+        <v>14</v>
+      </c>
     </row>
     <row r="13" spans="1:16" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="15"/>
-      <c r="B13" s="7"/>
-      <c r="C13" s="7"/>
-      <c r="D13" s="8"/>
-      <c r="E13" s="15"/>
-      <c r="F13" s="16"/>
-      <c r="G13" s="15"/>
-      <c r="H13" s="17"/>
-      <c r="I13" s="10"/>
-      <c r="J13" s="6"/>
-      <c r="K13" s="15"/>
-      <c r="L13" s="6"/>
+      <c r="B13" s="18" t="s">
+        <v>13</v>
+      </c>
+      <c r="C13" s="18" t="s">
+        <v>12</v>
+      </c>
+      <c r="D13" s="19" t="str">
+        <f t="shared" si="0"/>
+        <v>Digikey Cart</v>
+      </c>
+      <c r="E13" s="24" t="s">
+        <v>50</v>
+      </c>
+      <c r="F13" s="25">
+        <v>3</v>
+      </c>
+      <c r="G13" s="24" t="s">
+        <v>36</v>
+      </c>
+      <c r="H13" s="26">
+        <v>0.1</v>
+      </c>
+      <c r="I13" s="23">
+        <f>Table1[[#This Row],[Price/unit]]*Table1[[#This Row],[Units]]</f>
+        <v>0.30000000000000004</v>
+      </c>
+      <c r="J13" s="20" t="s">
+        <v>56</v>
+      </c>
+      <c r="K13" s="19" t="s">
+        <v>78</v>
+      </c>
+      <c r="L13" s="6" t="s">
+        <v>14</v>
+      </c>
     </row>
     <row r="14" spans="1:16" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="15"/>
-      <c r="B14" s="7"/>
-      <c r="C14" s="7"/>
-      <c r="D14" s="8"/>
-      <c r="E14" s="15"/>
-      <c r="F14" s="16"/>
-      <c r="G14" s="15"/>
-      <c r="H14" s="17"/>
-      <c r="I14" s="17"/>
-      <c r="J14" s="6"/>
-      <c r="K14" s="15"/>
-      <c r="L14" s="6"/>
+      <c r="B14" s="18" t="s">
+        <v>13</v>
+      </c>
+      <c r="C14" s="18" t="s">
+        <v>12</v>
+      </c>
+      <c r="D14" s="19" t="str">
+        <f t="shared" si="0"/>
+        <v>Digikey Cart</v>
+      </c>
+      <c r="E14" s="24" t="s">
+        <v>51</v>
+      </c>
+      <c r="F14" s="25">
+        <v>3</v>
+      </c>
+      <c r="G14" s="24" t="s">
+        <v>37</v>
+      </c>
+      <c r="H14" s="26">
+        <v>1.71</v>
+      </c>
+      <c r="I14" s="23">
+        <f>Table1[[#This Row],[Price/unit]]*Table1[[#This Row],[Units]]</f>
+        <v>5.13</v>
+      </c>
+      <c r="J14" s="20" t="s">
+        <v>56</v>
+      </c>
+      <c r="K14" s="19" t="s">
+        <v>79</v>
+      </c>
+      <c r="L14" s="6" t="s">
+        <v>14</v>
+      </c>
     </row>
     <row r="15" spans="1:16" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="15"/>
-      <c r="B15" s="7"/>
-      <c r="C15" s="7"/>
-      <c r="D15" s="8"/>
-      <c r="E15" s="15"/>
-      <c r="F15" s="16"/>
-      <c r="G15" s="15"/>
-      <c r="H15" s="17"/>
-      <c r="I15" s="17"/>
-      <c r="J15" s="6"/>
-      <c r="K15" s="15"/>
-      <c r="L15" s="6"/>
+      <c r="B15" s="18" t="s">
+        <v>13</v>
+      </c>
+      <c r="C15" s="18" t="s">
+        <v>12</v>
+      </c>
+      <c r="D15" s="19" t="str">
+        <f t="shared" si="0"/>
+        <v>Digikey Cart</v>
+      </c>
+      <c r="E15" s="24" t="s">
+        <v>52</v>
+      </c>
+      <c r="F15" s="25">
+        <v>6</v>
+      </c>
+      <c r="G15" s="24" t="s">
+        <v>38</v>
+      </c>
+      <c r="H15" s="26">
+        <v>0.47</v>
+      </c>
+      <c r="I15" s="23">
+        <f>Table1[[#This Row],[Price/unit]]*Table1[[#This Row],[Units]]</f>
+        <v>2.82</v>
+      </c>
+      <c r="J15" s="20" t="s">
+        <v>56</v>
+      </c>
+      <c r="K15" s="19" t="s">
+        <v>80</v>
+      </c>
+      <c r="L15" s="6" t="s">
+        <v>14</v>
+      </c>
     </row>
     <row r="16" spans="1:16" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="15"/>
-      <c r="B16" s="7"/>
-      <c r="C16" s="7"/>
-      <c r="D16" s="8"/>
-      <c r="E16" s="15"/>
-      <c r="F16" s="16"/>
-      <c r="G16" s="15"/>
-      <c r="H16" s="17"/>
-      <c r="I16" s="17"/>
-      <c r="J16" s="6"/>
-      <c r="K16" s="15"/>
-      <c r="L16" s="6"/>
+      <c r="B16" s="18" t="s">
+        <v>13</v>
+      </c>
+      <c r="C16" s="18" t="s">
+        <v>12</v>
+      </c>
+      <c r="D16" s="19" t="str">
+        <f t="shared" si="0"/>
+        <v>Digikey Cart</v>
+      </c>
+      <c r="E16" s="20" t="s">
+        <v>53</v>
+      </c>
+      <c r="F16" s="21">
+        <v>6</v>
+      </c>
+      <c r="G16" s="20" t="s">
+        <v>39</v>
+      </c>
+      <c r="H16" s="23">
+        <v>0.32</v>
+      </c>
+      <c r="I16" s="23">
+        <f>Table1[[#This Row],[Price/unit]]*Table1[[#This Row],[Units]]</f>
+        <v>1.92</v>
+      </c>
+      <c r="J16" s="20" t="s">
+        <v>56</v>
+      </c>
+      <c r="K16" s="19" t="s">
+        <v>81</v>
+      </c>
+      <c r="L16" s="6" t="s">
+        <v>14</v>
+      </c>
     </row>
     <row r="17" spans="1:12" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="15"/>
-      <c r="B17" s="7"/>
-      <c r="C17" s="7"/>
-      <c r="D17" s="8"/>
-      <c r="E17" s="15"/>
-      <c r="F17" s="16"/>
-      <c r="G17" s="15"/>
-      <c r="H17" s="17"/>
-      <c r="I17" s="17"/>
-      <c r="J17" s="6"/>
-      <c r="K17" s="15"/>
-      <c r="L17" s="6"/>
+      <c r="B17" s="18" t="s">
+        <v>13</v>
+      </c>
+      <c r="C17" s="18" t="s">
+        <v>12</v>
+      </c>
+      <c r="D17" s="19" t="str">
+        <f t="shared" si="0"/>
+        <v>Digikey Cart</v>
+      </c>
+      <c r="E17" s="20" t="s">
+        <v>54</v>
+      </c>
+      <c r="F17" s="21">
+        <v>3</v>
+      </c>
+      <c r="G17" s="20" t="s">
+        <v>40</v>
+      </c>
+      <c r="H17" s="23">
+        <v>1.43</v>
+      </c>
+      <c r="I17" s="23">
+        <f>Table1[[#This Row],[Price/unit]]*Table1[[#This Row],[Units]]</f>
+        <v>4.29</v>
+      </c>
+      <c r="J17" s="20" t="s">
+        <v>56</v>
+      </c>
+      <c r="K17" s="19" t="s">
+        <v>70</v>
+      </c>
+      <c r="L17" s="6" t="s">
+        <v>14</v>
+      </c>
     </row>
     <row r="18" spans="1:12" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="15"/>
-      <c r="B18" s="7"/>
-      <c r="C18" s="7"/>
-      <c r="D18" s="8"/>
-      <c r="E18" s="15"/>
-      <c r="F18" s="16"/>
-      <c r="G18" s="15"/>
-      <c r="H18" s="17"/>
-      <c r="I18" s="17"/>
-      <c r="J18" s="6"/>
-      <c r="K18" s="15"/>
-      <c r="L18" s="6"/>
+      <c r="B18" s="18" t="s">
+        <v>13</v>
+      </c>
+      <c r="C18" s="18" t="s">
+        <v>12</v>
+      </c>
+      <c r="D18" s="19" t="str">
+        <f t="shared" si="0"/>
+        <v>Digikey Cart</v>
+      </c>
+      <c r="E18" s="20" t="s">
+        <v>55</v>
+      </c>
+      <c r="F18" s="21">
+        <v>15</v>
+      </c>
+      <c r="G18" s="20" t="s">
+        <v>41</v>
+      </c>
+      <c r="H18" s="23">
+        <v>0.21299999999999999</v>
+      </c>
+      <c r="I18" s="23">
+        <f>Table1[[#This Row],[Price/unit]]*Table1[[#This Row],[Units]]</f>
+        <v>3.1949999999999998</v>
+      </c>
+      <c r="J18" s="20" t="s">
+        <v>56</v>
+      </c>
+      <c r="K18" s="19" t="s">
+        <v>71</v>
+      </c>
+      <c r="L18" s="6" t="s">
+        <v>14</v>
+      </c>
     </row>
     <row r="19" spans="1:12" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="15"/>
-      <c r="B19" s="7"/>
-      <c r="C19" s="7"/>
-      <c r="D19" s="8"/>
-      <c r="E19" s="15"/>
-      <c r="F19" s="16"/>
-      <c r="G19" s="15"/>
-      <c r="H19" s="17"/>
-      <c r="I19" s="17"/>
-      <c r="J19" s="6"/>
-      <c r="K19" s="15"/>
-      <c r="L19" s="6"/>
+      <c r="B19" s="18" t="s">
+        <v>13</v>
+      </c>
+      <c r="C19" s="18" t="s">
+        <v>12</v>
+      </c>
+      <c r="D19" s="19" t="str">
+        <f t="shared" si="0"/>
+        <v>Digikey Cart</v>
+      </c>
+      <c r="E19" s="24" t="s">
+        <v>63</v>
+      </c>
+      <c r="F19" s="25">
+        <v>10</v>
+      </c>
+      <c r="G19" s="24" t="s">
+        <v>64</v>
+      </c>
+      <c r="H19" s="26">
+        <v>0.73</v>
+      </c>
+      <c r="I19" s="26">
+        <f>Table1[[#This Row],[Price/unit]]*Table1[[#This Row],[Units]]</f>
+        <v>7.3</v>
+      </c>
+      <c r="J19" s="20" t="s">
+        <v>65</v>
+      </c>
+      <c r="K19" s="24" t="s">
+        <v>72</v>
+      </c>
+      <c r="L19" s="6" t="s">
+        <v>14</v>
+      </c>
     </row>
     <row r="20" spans="1:12" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="15"/>
-      <c r="B20" s="7"/>
-      <c r="C20" s="7"/>
-      <c r="D20" s="8"/>
-      <c r="E20" s="15"/>
-      <c r="F20" s="16"/>
-      <c r="G20" s="15"/>
-      <c r="H20" s="17"/>
-      <c r="I20" s="17"/>
-      <c r="J20" s="6"/>
-      <c r="K20" s="15"/>
-      <c r="L20" s="6"/>
+      <c r="B20" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="C20" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="D20" s="1" t="str">
+        <f>HYPERLINK("https://www.mouser.com/ProductDetail/Texas-Instruments/LMZM23601V5SILT?qs=W0yvOO0ixfFg%252Bmin1dyy1g%3D%3D","Mouser")</f>
+        <v>Mouser</v>
+      </c>
+      <c r="E20" s="6" t="s">
+        <v>57</v>
+      </c>
+      <c r="F20" s="9">
+        <v>5</v>
+      </c>
+      <c r="G20" s="6" t="s">
+        <v>59</v>
+      </c>
+      <c r="H20" s="10">
+        <v>6.47</v>
+      </c>
+      <c r="I20" s="17">
+        <f>Table1[[#This Row],[Price/unit]]*Table1[[#This Row],[Units]]</f>
+        <v>32.35</v>
+      </c>
+      <c r="J20" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="K20" s="15" t="s">
+        <v>61</v>
+      </c>
+      <c r="L20" s="6" t="s">
+        <v>14</v>
+      </c>
     </row>
     <row r="21" spans="1:12" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="15"/>
-      <c r="B21" s="7"/>
-      <c r="C21" s="7"/>
-      <c r="D21" s="8"/>
-      <c r="E21" s="15"/>
-      <c r="F21" s="16"/>
-      <c r="G21" s="15"/>
-      <c r="H21" s="17"/>
-      <c r="I21" s="17"/>
-      <c r="J21" s="6"/>
-      <c r="K21" s="15"/>
-      <c r="L21" s="6"/>
+      <c r="B21" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="C21" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="D21" s="1" t="str">
+        <f>HYPERLINK("https://www.amazon.com/BIGTREETECH-Printer-Stepstick-TMC2209-Heatsink/dp/B07YW7BM68/ref=sr_1_3?dchild=1&amp;keywords=TMC2209&amp;qid=1631245993&amp;sr=8-3","Amazon")</f>
+        <v>Amazon</v>
+      </c>
+      <c r="E21" s="6" t="s">
+        <v>58</v>
+      </c>
+      <c r="F21" s="9">
+        <v>1</v>
+      </c>
+      <c r="G21" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="H21" s="10">
+        <v>30.99</v>
+      </c>
+      <c r="I21" s="17">
+        <f>Table1[[#This Row],[Price/unit]]*Table1[[#This Row],[Units]]</f>
+        <v>30.99</v>
+      </c>
+      <c r="J21" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="K21" s="15" t="s">
+        <v>62</v>
+      </c>
+      <c r="L21" s="6" t="s">
+        <v>14</v>
+      </c>
     </row>
     <row r="22" spans="1:12" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="15"/>
-      <c r="B22" s="7"/>
-      <c r="C22" s="7"/>
-      <c r="D22" s="8"/>
-      <c r="E22" s="15"/>
-      <c r="F22" s="16"/>
-      <c r="G22" s="15"/>
-      <c r="H22" s="17"/>
-      <c r="I22" s="17"/>
-      <c r="J22" s="6"/>
+      <c r="B22" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="C22" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="D22" s="1" t="str">
+        <f>HYPERLINK("https://amzn.to/3tuGA9J","Amazon")</f>
+        <v>Amazon</v>
+      </c>
+      <c r="E22" s="15" t="s">
+        <v>66</v>
+      </c>
+      <c r="F22" s="16">
+        <v>1</v>
+      </c>
+      <c r="G22" s="15" t="s">
+        <v>67</v>
+      </c>
+      <c r="H22" s="17">
+        <v>11.98</v>
+      </c>
+      <c r="I22" s="17">
+        <f>Table1[[#This Row],[Price/unit]]*Table1[[#This Row],[Units]]</f>
+        <v>11.98</v>
+      </c>
+      <c r="J22" s="6" t="s">
+        <v>65</v>
+      </c>
       <c r="K22" s="15"/>
-      <c r="L22" s="6"/>
+      <c r="L22" s="6" t="s">
+        <v>14</v>
+      </c>
     </row>
     <row r="23" spans="1:12" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="15"/>
-      <c r="B23" s="7"/>
-      <c r="C23" s="7"/>
-      <c r="D23" s="8"/>
-      <c r="E23" s="15"/>
-      <c r="F23" s="16"/>
-      <c r="G23" s="15"/>
-      <c r="H23" s="17"/>
-      <c r="I23" s="17"/>
-      <c r="J23" s="6"/>
+      <c r="B23" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="C23" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="D23" s="1" t="str">
+        <f>HYPERLINK("https://amzn.to/3yWNpC3","Amazon")</f>
+        <v>Amazon</v>
+      </c>
+      <c r="E23" s="15" t="s">
+        <v>68</v>
+      </c>
+      <c r="F23" s="16">
+        <v>1</v>
+      </c>
+      <c r="G23" s="15" t="s">
+        <v>69</v>
+      </c>
+      <c r="H23" s="17">
+        <v>9.99</v>
+      </c>
+      <c r="I23" s="17">
+        <f>Table1[[#This Row],[Price/unit]]*Table1[[#This Row],[Units]]</f>
+        <v>9.99</v>
+      </c>
+      <c r="J23" s="6" t="s">
+        <v>65</v>
+      </c>
       <c r="K23" s="15"/>
       <c r="L23" s="6"/>
     </row>
-    <row r="24" spans="1:12" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A24" s="15"/>
       <c r="B24" s="7"/>
       <c r="C24" s="7"/>
@@ -1780,20 +2240,7 @@
       <c r="K24" s="15"/>
       <c r="L24" s="6"/>
     </row>
-    <row r="25" spans="1:12" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="15"/>
-      <c r="B25" s="7"/>
-      <c r="C25" s="7"/>
-      <c r="D25" s="8"/>
-      <c r="E25" s="15"/>
-      <c r="F25" s="16"/>
-      <c r="G25" s="15"/>
-      <c r="H25" s="17"/>
-      <c r="I25" s="17"/>
-      <c r="J25" s="6"/>
-      <c r="K25" s="15"/>
-      <c r="L25" s="6"/>
-    </row>
+    <row r="25" spans="1:12" ht="18.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="26" spans="1:12" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26" s="15"/>
       <c r="B26" s="7"/>
@@ -1804,7 +2251,7 @@
       <c r="G26" s="15"/>
       <c r="H26" s="17"/>
       <c r="I26" s="17"/>
-      <c r="J26" s="6"/>
+      <c r="J26" s="15"/>
       <c r="K26" s="15"/>
       <c r="L26" s="6"/>
     </row>
@@ -2046,7 +2493,7 @@
       <c r="K43" s="15"/>
       <c r="L43" s="6"/>
     </row>
-    <row r="44" spans="1:12" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A44" s="15"/>
       <c r="B44" s="7"/>
       <c r="C44" s="7"/>
@@ -2060,35 +2507,11 @@
       <c r="K44" s="15"/>
       <c r="L44" s="6"/>
     </row>
-    <row r="45" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A45" s="15"/>
-      <c r="B45" s="7"/>
-      <c r="C45" s="7"/>
-      <c r="D45" s="8"/>
-      <c r="E45" s="15"/>
-      <c r="F45" s="16"/>
-      <c r="G45" s="15"/>
-      <c r="H45" s="17"/>
-      <c r="I45" s="17"/>
-      <c r="J45" s="15"/>
-      <c r="K45" s="15"/>
-      <c r="L45" s="6"/>
-    </row>
   </sheetData>
-  <hyperlinks>
-    <hyperlink ref="K2" r:id="rId1" xr:uid="{7E6902C0-DA9E-4F01-B2C2-D7E01FF8578A}"/>
-    <hyperlink ref="K3" r:id="rId2" xr:uid="{F3C40A91-B1F7-4D9E-87B2-8DC270EC6A75}"/>
-    <hyperlink ref="K4" r:id="rId3" xr:uid="{F78CE6C1-C7C7-4C16-B917-B5E8DD3CE34D}"/>
-    <hyperlink ref="K5" r:id="rId4" xr:uid="{9EB82BD5-F63C-451D-9C3F-3A3E17AA506B}"/>
-    <hyperlink ref="K6" r:id="rId5" xr:uid="{F5D926A3-671B-48F1-94B6-661F55AEB5AA}"/>
-    <hyperlink ref="K7" r:id="rId6" xr:uid="{169EBBFA-0A8B-408E-B793-AEE0227A1685}"/>
-    <hyperlink ref="K8" r:id="rId7" xr:uid="{8776012F-8B7F-4043-912B-E7152288CA2A}"/>
-    <hyperlink ref="K9" r:id="rId8" xr:uid="{5DB5FF92-2D5A-4213-866F-AAC89A563D5A}"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId9"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
   <tableParts count="1">
-    <tablePart r:id="rId10"/>
+    <tablePart r:id="rId2"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>